<commit_message>
Upated scripts with comments
</commit_message>
<xml_diff>
--- a/API_Results.xlsx
+++ b/API_Results.xlsx
@@ -15,16 +15,75 @@
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>HardDisk</t>
+  </si>
+  <si>
+    <t>CreatedAt</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>ff8081819782e69e0199083b378715dd</t>
+  </si>
+  <si>
+    <t>Apple MacBook Pro 18 Max</t>
+  </si>
+  <si>
+    <t>Intel Core i8</t>
+  </si>
+  <si>
+    <t>4 TB</t>
+  </si>
+  <si>
+    <t>2025-09-02T02:22:02.631+00:00</t>
+  </si>
+  <si>
+    <t>2025-09-02 07:52:02</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>ff8081819782e69e0199083a69e415da</t>
+  </si>
+  <si>
+    <t>2025-09-02 07:51:10</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -57,9 +116,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="22" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="A1:I13"/>
@@ -382,35 +441,132 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="52.453125" customWidth="1"/>
-    <col min="3" max="3" width="52.81640625" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="44.81640625" customWidth="1"/>
-    <col min="9" max="9" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.4612627029419" customWidth="1"/>
+    <col min="2" max="2" width="53.0742607116699" customWidth="1"/>
+    <col min="3" max="3" width="38.1595039367676" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7822723388672" customWidth="1"/>
+    <col min="6" max="6" width="17.7355365753174" customWidth="1"/>
+    <col min="7" max="7" width="13.9711675643921" customWidth="1"/>
+    <col min="8" max="8" width="44.7997093200684" customWidth="1"/>
+    <col min="9" max="9" width="29.1744289398193" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="I2" s="1"/>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0">
+        <v>2021</v>
+      </c>
+      <c r="E2" s="0">
+        <v>189.99</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5">
       <c r="I5" s="1"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="0">
+        <v>2021</v>
+      </c>
+      <c r="E6" s="0">
+        <v>189.99</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0">
+        <v>2021</v>
+      </c>
+      <c r="E7" s="0">
+        <v>189.99</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>